<commit_message>
optimize error handling in worker.js, fix README.md, optimize test dats files
</commit_message>
<xml_diff>
--- a/assets/data/basis.xlsx
+++ b/assets/data/basis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisstark/Documents/IntelliJ_Projects/File-Compare/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisstark/Documents/IntelliJ_Projects/file-compare/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428522A-B95D-134F-84E8-93C19CEE4866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41E9570-0B4A-4741-B68F-6B0BDBAC812A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52640" yWindow="1600" windowWidth="28040" windowHeight="17440" xr2:uid="{2158DCE0-E3CF-0640-AA0D-70E629025B45}"/>
   </bookViews>
@@ -37,18 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Alter</t>
-  </si>
-  <si>
-    <t>Stadt</t>
-  </si>
-  <si>
     <t>Anna</t>
   </si>
   <si>
@@ -104,13 +92,25 @@
   </si>
   <si>
     <t>Dresden</t>
+  </si>
+  <si>
+    <t>Customer Number</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,13 +121,14 @@
     <font>
       <sz val="13"/>
       <color rgb="FF0E0E0E"/>
-      <name val=".SF NS"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF0E0E0E"/>
-      <name val=".SF NS"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,8 +153,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,163 +472,166 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C4" s="2">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" s="2">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C6" s="2">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C7" s="2">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C8" s="2">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C9" s="2">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C10" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C11" s="2">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C9">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>